<commit_message>
Many Mini CPU Bug Fix
</commit_message>
<xml_diff>
--- a/Opcodes.xlsx
+++ b/Opcodes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Cool Stuffy Stuffs\Gameboy Detonation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cool Stuffy Stuffs\Gameboy-Detonation (git)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC1E973-7661-47EE-8E30-2052E262A15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233383C2-7F5B-4BF0-9B60-DABFC88E6698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{17B713DC-27D0-419D-9B78-A3C59C1AD0E7}"/>
   </bookViews>
@@ -786,7 +786,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -801,25 +801,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -851,38 +833,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1201,7 +1171,7 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,49 +1251,49 @@
         <f>DEC2HEX(0*16, 2)</f>
         <v>00</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>97</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="2" t="s">
         <v>215</v>
       </c>
       <c r="Q2" s="2" t="s">
@@ -1335,49 +1305,49 @@
         <f>DEC2HEX(HEX2DEC(A2)+16, 2)</f>
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>98</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="P3" s="2" t="s">
         <v>216</v>
       </c>
       <c r="Q3" s="2" t="s">
@@ -1389,52 +1359,52 @@
         <f t="shared" ref="A4:A15" si="1">DEC2HEX(HEX2DEC(A3)+16, 2)</f>
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="P4" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="Q4" s="2" t="s">
         <v>233</v>
       </c>
     </row>
@@ -1443,52 +1413,52 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="2" t="s">
         <v>234</v>
       </c>
     </row>
@@ -1497,52 +1467,52 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="L6" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="O6" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="P6" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" s="2" t="s">
         <v>235</v>
       </c>
     </row>
@@ -1551,52 +1521,52 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="2" t="s">
         <v>236</v>
       </c>
     </row>
@@ -1605,52 +1575,52 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="M8" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="O8" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="P8" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="2" t="s">
         <v>237</v>
       </c>
     </row>
@@ -1659,52 +1629,52 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="O9" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="Q9" s="2" t="s">
         <v>238</v>
       </c>
     </row>
@@ -1713,28 +1683,28 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="2" t="s">
         <v>120</v>
       </c>
       <c r="J10" s="2" t="s">
@@ -1767,28 +1737,28 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="2" t="s">
         <v>121</v>
       </c>
       <c r="J11" s="2" t="s">
@@ -1821,52 +1791,52 @@
         <f t="shared" si="1"/>
         <v>A0</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="L12" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="M12" s="5" t="s">
+      <c r="M12" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="O12" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="P12" s="5" t="s">
+      <c r="P12" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="Q12" s="5" t="s">
+      <c r="Q12" s="2" t="s">
         <v>196</v>
       </c>
     </row>
@@ -1875,52 +1845,52 @@
         <f t="shared" si="1"/>
         <v>B0</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="L13" s="5" t="s">
+      <c r="L13" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="M13" s="5" t="s">
+      <c r="M13" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="O13" s="5" t="s">
+      <c r="O13" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="P13" s="5" t="s">
+      <c r="P13" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="Q13" s="5" t="s">
+      <c r="Q13" s="2" t="s">
         <v>240</v>
       </c>
     </row>
@@ -1929,52 +1899,52 @@
         <f t="shared" si="1"/>
         <v>C0</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M14" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="N14" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="O14" s="6" t="s">
+      <c r="O14" s="2" t="s">
         <v>212</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="Q14" s="6" t="s">
+      <c r="Q14" s="2" t="s">
         <v>241</v>
       </c>
     </row>
@@ -1983,46 +1953,46 @@
         <f t="shared" si="1"/>
         <v>D0</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="7" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="K15" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="L15" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="6" t="s">
+      <c r="M15" s="4"/>
+      <c r="N15" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="O15" s="5"/>
+      <c r="O15" s="4"/>
       <c r="P15" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="Q15" s="6" t="s">
+      <c r="Q15" s="2" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2031,42 +2001,42 @@
         <f>DEC2HEX(HEX2DEC(A15)+16, 2)</f>
         <v>E0</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="1" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5" t="s">
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="Q16" s="6" t="s">
+      <c r="Q16" s="2" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2075,46 +2045,46 @@
         <f>DEC2HEX(HEX2DEC(A16)+16, 2)</f>
         <v>F0</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="1" t="s">
+      <c r="F17" s="4"/>
+      <c r="G17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="M17" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5" t="s">
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="Q17" s="6" t="s">
+      <c r="Q17" s="2" t="s">
         <v>244</v>
       </c>
     </row>
@@ -2189,352 +2159,352 @@
         <f>DEC2HEX(0*16, 2)</f>
         <v>00</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
     </row>
     <row r="22" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>DEC2HEX(HEX2DEC(A21)+16, 2)</f>
         <v>10</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
     </row>
     <row r="23" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" ref="A23:A34" si="3">DEC2HEX(HEX2DEC(A22)+16, 2)</f>
         <v>20</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
     </row>
     <row r="24" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
     </row>
     <row r="25" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
     </row>
     <row r="26" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
     </row>
     <row r="28" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
     </row>
     <row r="29" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
     </row>
     <row r="30" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
     </row>
     <row r="31" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f t="shared" si="3"/>
         <v>A0</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
     </row>
     <row r="32" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f t="shared" si="3"/>
         <v>B0</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
     </row>
     <row r="33" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f t="shared" si="3"/>
         <v>C0</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
     </row>
     <row r="34" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f t="shared" si="3"/>
         <v>D0</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
     </row>
     <row r="35" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>DEC2HEX(HEX2DEC(A34)+16, 2)</f>
         <v>E0</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
     </row>
     <row r="36" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>DEC2HEX(HEX2DEC(A35)+16, 2)</f>
         <v>F0</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>